<commit_message>
Test fixes, results tweaks
</commit_message>
<xml_diff>
--- a/inst/models/example_markov/model.xlsx
+++ b/inst/models/example_markov/model.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t xml:space="preserve">setting</t>
   </si>
@@ -438,6 +438,36 @@
   </si>
   <si>
     <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">seritinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seritinib</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volantor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volantor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cendralimab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cendralimab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gamma(mean = 5000, sd = 1000)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lognormal(mean = 0.4, sd = 0.08)</t>
   </si>
 </sst>
 </file>
@@ -929,18 +959,26 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1558,7 +1596,7 @@
         <v>76</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="E9"/>
       <c r="F9" t="s">
@@ -1580,7 +1618,7 @@
         <v>77</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="E10"/>
       <c r="F10" t="s">
@@ -1602,7 +1640,7 @@
         <v>61</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="E11"/>
       <c r="F11"/>
@@ -1622,7 +1660,7 @@
         <v>80</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>141</v>
       </c>
       <c r="E12"/>
       <c r="F12" t="s">
@@ -1764,6 +1802,50 @@
         <v>57</v>
       </c>
       <c r="H18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" t="s">
+        <v>143</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" t="s">
+        <v>75</v>
+      </c>
+      <c r="H19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>